<commit_message>
Fix para winrate. Ahora se muestra el procentaje en la grafica, MEJORADO sin bugs
</commit_message>
<xml_diff>
--- a/src/ar/edu/unrc/game2048/resources/Estadisticas.xlsx
+++ b/src/ar/edu/unrc/game2048/resources/Estadisticas.xlsx
@@ -344,9 +344,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0%"/>
+    <numFmt numFmtId="166" formatCode="0.00%"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -445,7 +446,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -463,6 +464,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -12300,11 +12305,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="37196712"/>
-        <c:axId val="62905891"/>
+        <c:axId val="62910238"/>
+        <c:axId val="31052176"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="37196712"/>
+        <c:axId val="62910238"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12320,14 +12325,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="62905891"/>
+        <c:crossAx val="31052176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="62905891"/>
+        <c:axId val="31052176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12352,7 +12357,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="37196712"/>
+        <c:crossAx val="62910238"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -29477,11 +29482,11 @@
           <c:downBars/>
         </c:upDownBars>
         <c:marker val="1"/>
-        <c:axId val="33438394"/>
-        <c:axId val="10521630"/>
+        <c:axId val="53243944"/>
+        <c:axId val="58450744"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="33438394"/>
+        <c:axId val="53243944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -29497,14 +29502,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="10521630"/>
+        <c:crossAx val="58450744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="10521630"/>
+        <c:axId val="58450744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -29529,7 +29534,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="33438394"/>
+        <c:crossAx val="53243944"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -41591,11 +41596,11 @@
           <c:downBars/>
         </c:upDownBars>
         <c:marker val="1"/>
-        <c:axId val="55658170"/>
-        <c:axId val="93744241"/>
+        <c:axId val="84005032"/>
+        <c:axId val="33760110"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="55658170"/>
+        <c:axId val="84005032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -41611,14 +41616,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="93744241"/>
+        <c:crossAx val="33760110"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93744241"/>
+        <c:axId val="33760110"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -41643,7 +41648,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="55658170"/>
+        <c:crossAx val="84005032"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -43645,11 +43650,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="17776748"/>
-        <c:axId val="47203985"/>
+        <c:axId val="70572896"/>
+        <c:axId val="85737888"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="17776748"/>
+        <c:axId val="70572896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -43665,14 +43670,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="47203985"/>
+        <c:crossAx val="85737888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="47203985"/>
+        <c:axId val="85737888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -43697,7 +43702,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="17776748"/>
+        <c:crossAx val="70572896"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -51732,11 +51737,11 @@
           <c:downBars/>
         </c:upDownBars>
         <c:marker val="1"/>
-        <c:axId val="4292684"/>
-        <c:axId val="19428126"/>
+        <c:axId val="68349012"/>
+        <c:axId val="58367942"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="4292684"/>
+        <c:axId val="68349012"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -51752,14 +51757,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="19428126"/>
+        <c:crossAx val="58367942"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="19428126"/>
+        <c:axId val="58367942"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -51784,7 +51789,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="4292684"/>
+        <c:crossAx val="68349012"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -53841,11 +53846,11 @@
           <c:downBars/>
         </c:upDownBars>
         <c:marker val="1"/>
-        <c:axId val="54798293"/>
-        <c:axId val="53970994"/>
+        <c:axId val="74415832"/>
+        <c:axId val="92261213"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="54798293"/>
+        <c:axId val="74415832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -53861,14 +53866,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="53970994"/>
+        <c:crossAx val="92261213"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53970994"/>
+        <c:axId val="92261213"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -53893,7 +53898,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="54798293"/>
+        <c:crossAx val="74415832"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -54296,7 +54301,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
                 <c:pt idx="0">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v/>
@@ -54616,11 +54621,11 @@
           <c:downBars/>
         </c:upDownBars>
         <c:marker val="1"/>
-        <c:axId val="5486696"/>
-        <c:axId val="51766607"/>
+        <c:axId val="62342501"/>
+        <c:axId val="77011442"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="5486696"/>
+        <c:axId val="62342501"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -54636,14 +54641,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="51766607"/>
+        <c:crossAx val="77011442"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51766607"/>
+        <c:axId val="77011442"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -54677,7 +54682,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="5486696"/>
+        <c:crossAx val="62342501"/>
         <c:crossesAt val="1"/>
       </c:valAx>
       <c:spPr>
@@ -54717,15 +54722,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>81000</xdr:colOff>
+      <xdr:colOff>162000</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>74520</xdr:rowOff>
+      <xdr:rowOff>47520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>15840</xdr:colOff>
+      <xdr:colOff>95760</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>151560</xdr:rowOff>
+      <xdr:rowOff>123480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -54733,8 +54738,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="81000" y="3162960"/>
-        <a:ext cx="8042400" cy="5279040"/>
+        <a:off x="162000" y="3135960"/>
+        <a:ext cx="8041320" cy="5277960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -54747,15 +54752,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>4320</xdr:colOff>
+      <xdr:colOff>85320</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>122400</xdr:rowOff>
+      <xdr:rowOff>95400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>36</xdr:col>
-      <xdr:colOff>30600</xdr:colOff>
+      <xdr:colOff>110520</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>153000</xdr:rowOff>
+      <xdr:rowOff>124920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -54763,8 +54768,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8111880" y="3210840"/>
-        <a:ext cx="10797840" cy="5069880"/>
+        <a:off x="8192880" y="3183840"/>
+        <a:ext cx="10796760" cy="5068800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -54777,15 +54782,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>84600</xdr:colOff>
+      <xdr:colOff>165600</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>116640</xdr:rowOff>
+      <xdr:rowOff>89640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>106560</xdr:colOff>
+      <xdr:colOff>186480</xdr:colOff>
       <xdr:row>78</xdr:row>
-      <xdr:rowOff>39240</xdr:rowOff>
+      <xdr:rowOff>11160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -54793,8 +54798,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="84600" y="8244360"/>
-        <a:ext cx="16744680" cy="4474440"/>
+        <a:off x="165600" y="8217360"/>
+        <a:ext cx="16743600" cy="4473360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -54812,15 +54817,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>94680</xdr:colOff>
+      <xdr:colOff>175680</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>56160</xdr:rowOff>
+      <xdr:rowOff>29160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>29880</xdr:colOff>
+      <xdr:colOff>109800</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>132840</xdr:rowOff>
+      <xdr:rowOff>104760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -54828,8 +54833,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="94680" y="706320"/>
-        <a:ext cx="8195040" cy="5278680"/>
+        <a:off x="175680" y="679320"/>
+        <a:ext cx="8193960" cy="5277600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -54842,15 +54847,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>297000</xdr:colOff>
+      <xdr:colOff>378000</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:rowOff>18720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>34</xdr:col>
-      <xdr:colOff>397080</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>3240</xdr:rowOff>
+      <xdr:colOff>477000</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>137880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -54858,8 +54863,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7541640" y="695880"/>
-        <a:ext cx="10797840" cy="4996800"/>
+        <a:off x="7622640" y="668880"/>
+        <a:ext cx="10796760" cy="4995720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -54872,15 +54877,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>91080</xdr:colOff>
+      <xdr:colOff>172080</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>87480</xdr:rowOff>
+      <xdr:rowOff>60480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>342720</xdr:colOff>
+      <xdr:colOff>422640</xdr:colOff>
       <xdr:row>63</xdr:row>
-      <xdr:rowOff>95760</xdr:rowOff>
+      <xdr:rowOff>67680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -54888,8 +54893,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="91080" y="5939640"/>
-        <a:ext cx="17126640" cy="4397400"/>
+        <a:off x="172080" y="5912640"/>
+        <a:ext cx="17125560" cy="4396320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -54907,15 +54912,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>131040</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>11520</xdr:rowOff>
+      <xdr:colOff>212040</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>146880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>382680</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>19800</xdr:rowOff>
+      <xdr:colOff>462600</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>154080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -54923,8 +54928,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="131040" y="498960"/>
-        <a:ext cx="17126640" cy="4397400"/>
+        <a:off x="212040" y="471960"/>
+        <a:ext cx="17125560" cy="4396320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -57997,7 +58002,7 @@
   <dimension ref="B1:CY2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H36" activeCellId="0" sqref="H36"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -58357,107 +58362,109 @@
       <c r="B2" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
-      <c r="Y2" s="4"/>
-      <c r="Z2" s="4"/>
-      <c r="AA2" s="4"/>
-      <c r="AB2" s="4"/>
-      <c r="AC2" s="4"/>
-      <c r="AD2" s="4"/>
-      <c r="AE2" s="4"/>
-      <c r="AF2" s="4"/>
-      <c r="AG2" s="4"/>
-      <c r="AH2" s="4"/>
-      <c r="AI2" s="4"/>
-      <c r="AJ2" s="4"/>
-      <c r="AK2" s="4"/>
-      <c r="AL2" s="4"/>
-      <c r="AM2" s="4"/>
-      <c r="AN2" s="4"/>
-      <c r="AO2" s="4"/>
-      <c r="AP2" s="4"/>
-      <c r="AQ2" s="4"/>
-      <c r="AR2" s="4"/>
-      <c r="AS2" s="4"/>
-      <c r="AT2" s="4"/>
-      <c r="AU2" s="4"/>
-      <c r="AV2" s="4"/>
-      <c r="AW2" s="4"/>
-      <c r="AX2" s="4"/>
-      <c r="AY2" s="4"/>
-      <c r="AZ2" s="4"/>
-      <c r="BA2" s="4"/>
-      <c r="BB2" s="4"/>
-      <c r="BC2" s="4"/>
-      <c r="BD2" s="4"/>
-      <c r="BE2" s="4"/>
-      <c r="BF2" s="4"/>
-      <c r="BG2" s="4"/>
-      <c r="BH2" s="4"/>
-      <c r="BI2" s="4"/>
-      <c r="BJ2" s="4"/>
-      <c r="BK2" s="4"/>
-      <c r="BL2" s="4"/>
-      <c r="BM2" s="4"/>
-      <c r="BN2" s="4"/>
-      <c r="BO2" s="4"/>
-      <c r="BP2" s="4"/>
-      <c r="BQ2" s="4"/>
-      <c r="BR2" s="4"/>
-      <c r="BS2" s="4"/>
-      <c r="BT2" s="4"/>
-      <c r="BU2" s="4"/>
-      <c r="BV2" s="4"/>
-      <c r="BW2" s="4"/>
-      <c r="BX2" s="4"/>
-      <c r="BY2" s="4"/>
-      <c r="BZ2" s="4"/>
-      <c r="CA2" s="4"/>
-      <c r="CB2" s="4"/>
-      <c r="CC2" s="4"/>
-      <c r="CD2" s="4"/>
-      <c r="CE2" s="4"/>
-      <c r="CF2" s="4"/>
-      <c r="CG2" s="4"/>
-      <c r="CH2" s="4"/>
-      <c r="CI2" s="4"/>
-      <c r="CJ2" s="4"/>
-      <c r="CK2" s="4"/>
-      <c r="CL2" s="4"/>
-      <c r="CM2" s="4"/>
-      <c r="CN2" s="4"/>
-      <c r="CO2" s="4"/>
-      <c r="CP2" s="4"/>
-      <c r="CQ2" s="4"/>
-      <c r="CR2" s="4"/>
-      <c r="CS2" s="4"/>
-      <c r="CT2" s="4"/>
-      <c r="CU2" s="4"/>
-      <c r="CV2" s="4"/>
-      <c r="CW2" s="4"/>
-      <c r="CX2" s="4"/>
-      <c r="CY2" s="4"/>
+      <c r="C2" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="5"/>
+      <c r="AB2" s="5"/>
+      <c r="AC2" s="5"/>
+      <c r="AD2" s="5"/>
+      <c r="AE2" s="5"/>
+      <c r="AF2" s="5"/>
+      <c r="AG2" s="5"/>
+      <c r="AH2" s="5"/>
+      <c r="AI2" s="5"/>
+      <c r="AJ2" s="5"/>
+      <c r="AK2" s="5"/>
+      <c r="AL2" s="5"/>
+      <c r="AM2" s="5"/>
+      <c r="AN2" s="5"/>
+      <c r="AO2" s="5"/>
+      <c r="AP2" s="5"/>
+      <c r="AQ2" s="5"/>
+      <c r="AR2" s="5"/>
+      <c r="AS2" s="5"/>
+      <c r="AT2" s="5"/>
+      <c r="AU2" s="5"/>
+      <c r="AV2" s="5"/>
+      <c r="AW2" s="5"/>
+      <c r="AX2" s="5"/>
+      <c r="AY2" s="5"/>
+      <c r="AZ2" s="5"/>
+      <c r="BA2" s="5"/>
+      <c r="BB2" s="5"/>
+      <c r="BC2" s="5"/>
+      <c r="BD2" s="5"/>
+      <c r="BE2" s="5"/>
+      <c r="BF2" s="5"/>
+      <c r="BG2" s="5"/>
+      <c r="BH2" s="5"/>
+      <c r="BI2" s="5"/>
+      <c r="BJ2" s="5"/>
+      <c r="BK2" s="5"/>
+      <c r="BL2" s="5"/>
+      <c r="BM2" s="5"/>
+      <c r="BN2" s="5"/>
+      <c r="BO2" s="5"/>
+      <c r="BP2" s="5"/>
+      <c r="BQ2" s="5"/>
+      <c r="BR2" s="5"/>
+      <c r="BS2" s="5"/>
+      <c r="BT2" s="5"/>
+      <c r="BU2" s="5"/>
+      <c r="BV2" s="5"/>
+      <c r="BW2" s="5"/>
+      <c r="BX2" s="5"/>
+      <c r="BY2" s="5"/>
+      <c r="BZ2" s="5"/>
+      <c r="CA2" s="5"/>
+      <c r="CB2" s="5"/>
+      <c r="CC2" s="5"/>
+      <c r="CD2" s="5"/>
+      <c r="CE2" s="5"/>
+      <c r="CF2" s="5"/>
+      <c r="CG2" s="5"/>
+      <c r="CH2" s="5"/>
+      <c r="CI2" s="5"/>
+      <c r="CJ2" s="5"/>
+      <c r="CK2" s="5"/>
+      <c r="CL2" s="5"/>
+      <c r="CM2" s="5"/>
+      <c r="CN2" s="5"/>
+      <c r="CO2" s="5"/>
+      <c r="CP2" s="5"/>
+      <c r="CQ2" s="5"/>
+      <c r="CR2" s="5"/>
+      <c r="CS2" s="5"/>
+      <c r="CT2" s="5"/>
+      <c r="CU2" s="5"/>
+      <c r="CV2" s="5"/>
+      <c r="CW2" s="5"/>
+      <c r="CX2" s="5"/>
+      <c r="CY2" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>